<commit_message>
Release 2024-03: Excel files ready for translation
</commit_message>
<xml_diff>
--- a/i18n/excel_to_translation/com.ipmwise.xlsx
+++ b/i18n/excel_to_translation/com.ipmwise.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="114">
   <si>
     <t>KEY</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>IPMwise</t>
+  </si>
+  <si>
+    <t>IMPwise</t>
   </si>
   <si>
     <t>com.ipmwise.4.models.ipmwiseDEMO.description</t>
@@ -97,6 +100,114 @@
   </si>
   <si>
     <t>Weed treatment advice</t>
+  </si>
+  <si>
+    <t>Tilpas ukrudtshåndteringen til dine behov som professionel landmand eller konsulent. Bestem selv niveauet af ukrudtsbekæmpelse, eller lad de indbyggede IPM-principper i IPMwise guide dig. Softwaren indeholder nyttige værktøjer til at tilpasse ukrudtsbekæmpelsen til den aktuelle ukrudtspopulation på en mark og dermed minimere brugen af ​​herbicider. Softwaren kan bruges til at planlægge herbicidoperationer på både markniveau og som et generelt planlægningsværktøj for rådgivere til at finde passende tankblandinger og tilsvarende mængder. Principperne for programmet er baseret på dosis-respons-data afledt af effektforsøg. I Danmark arbejdes der i øjeblikket på også at bruge beslutningsstøtteprogrammet IPMwise i kombination med kunstig intelligens, automatisk ukrudtsgenkendelse og bekæmpelseskort. Denne demo har været begrænset i forhold til antallet af afgrøder og ukrudt i forhold til den fulde danske version.</t>
+  </si>
+  <si>
+    <t>Råd om ukrudtsbekæmpelse</t>
+  </si>
+  <si>
+    <t>Passt das Unkrautmanagement an Ihre Bedürfnisse als professioneller Landwirt oder Anbauberater an. Entscheiden Sie selbst über den Grad der Unkrautbekämpfung oder lassen Sie sich von den integrierten IPM-Grundsätzen von IPMwise leiten. Die Software enthält nützliche Werkzeuge zur Anpassung der Unkrautbekämpfung an die Unkrautpopulation in einem Feld, um so den Einsatz von Herbiziden erheblich zu minimieren. Die Software kann sowohl zur Planung des Herbizideinsatzes auf Feldebene als auch als allgemeines Planungsinstrument für Pflanzenbauberater verwendet werden, um geeignete Tankmischungen und entsprechende Dosierungen zu finden. Die Grundsätze des Programms beruhen auf Dosis-Wirkungs-Daten, die aus Wirksamkeitsberichten abgeleitet werden. In Dänemark wird derzeit daran gearbeitet, die IPMwise-Entscheidungshilfe-Software in Verbindung mit künstlicher Intelligenz, automatischer Unkrauterkennung und Spritzkarten einzusetzen. Diese Demo ist hinsichtlich der Anzahl der Kulturen und Unkräuter im Vergleich zur dänischen Vollversion eingeschränkt.</t>
+  </si>
+  <si>
+    <t>IPMwise Demoversion</t>
+  </si>
+  <si>
+    <t>Beratung zur Unkrautbehandlung</t>
+  </si>
+  <si>
+    <t>Stem het onkruidbeheer af op uw behoeften als professionele landbouwer of gewasadviseur. Bepaal zelf het niveau van onkruidbestrijding of laat u leiden door de ingebouwde IPM-beginselen van IPMwise. Het programma bevat nuttige hulpmiddelen om de inspanning tegen onkruid aan te passen aan de huidige onkruidpopulatie in een veld en zo het gebruik van herbiciden aanzienlijk te minimaliseren. Het programma kan worden gebruikt voor het plannen van herbiciden bespuitingen op zowel veldniveau als voor een algemene planningstool voor gewasadviseurs om geschikte tankmixen en bijbehorende doseringen te vinden. 
+De uitgangspunten van het programma zijn gebaseerd op doseringsgegevens uit effectiviteitsrapporten. In Denemarken wordt momenteel gewerkt aan 
+het programma ook te gebruiken in combinatie met kunstmatige intelligentie, automatische onkruidherkenning en spuitkaarten. Deze demo is beperkt wat betreft het aantal gewassen en onkruiden in vergelijking met de volledige Deense versie.</t>
+  </si>
+  <si>
+    <t>IPMwise demo versie</t>
+  </si>
+  <si>
+    <t>Onkruidbestrijdingsadvies</t>
+  </si>
+  <si>
+    <t>Prilagodite obvladovanje plevela svojim potrebam. Sami se odločite o stopnji zatiranja plevela, ali pa se prepustite vgrajenim načelom IPMwise. Programska oprema vsebuje uporabna orodja, s katerimi lahko ukrep proti plevelu prilagodite trenutni stopnji zapleveljenosti in tako znatno zmanjšate uporabo herbicidov. Programsko opremo lahko uporabite za načrtovanje tretiranja s herbicidi tako na ravni polja ali kot splošno orodje za načrtovanje primerne škropilne mešanice in ustrezne odmerke za kmetijske svetovalce. Načela orodja temeljijo na podatkih o odzivu na odmerek, pridobljenih iz poročil o učinkovitosti. Na Danskem trenutno poteka delo za uporabo sistema za podporo odločanju IPMwise v povezavi z umetno inteligenco, samodejnim prepoznavanjem plevela in zemljevidi škropljenja. Ta demo različica je bila v primerjavi s polno dansko različico omejena glede števila poljščin in plevelov.</t>
+  </si>
+  <si>
+    <t>Demo različica programa IPMwise</t>
+  </si>
+  <si>
+    <t>Nasveti za zatiranje plevela</t>
+  </si>
+  <si>
+    <t>Tilpass ugrashåndteringen til dine behov som profesjonell bonde eller avlingsrådgiver. Du kan selv bestemme nivået av ugrasbekjempelse, eller la de innebygde IPV-prinsippene i IPMwise veilede deg. Programvaren inneholder nyttige verktøy for å tilpasse innsatsen mot ugras til den nåværende ugrasbestand i en åker og dermed minimere bruken av herbicider betraktelig. Programvaren kan brukes til å planlegge bruken av herbicider både på feltnivå og som et generelt planleggingsverktøy for avlingsrådgivere for å finne passende blandinger og tilsvarende doseringsrater. Prinsippene for programmet er basert på doseresponsdata utledet fra effektrapporter. I Danmark jobbes det for tiden med å bruke IPMwise programvare beslutningsstøtte i forbindelse med kunstig intelligens, automatisk ugrasgjenkjenning og sprøytekart. Denne demoen har vært begrenset med hensyn til antall avlinger og ugras sammenlignet med den fullstendige danske versjonen.</t>
+  </si>
+  <si>
+    <t>Demoversjon av IPMwise</t>
+  </si>
+  <si>
+    <t>Råd om bekjempelse av ugras</t>
+  </si>
+  <si>
+    <t>Anpassa ogräshanteringen efter dina behov som professionell lantbrukare eller rådgivare. Bestäm själv nivån på ogräsbekämpning eller låt de inbyggda IPM-principerna i IPMwise vägleda dig. Programvaran innehåller användbara verktyg för att anpassa ogräsbekämpningen till den aktuella ogräspopulationen i ett fält och därmed en minimerad användning av herbicider. Programvaran kan användas för att planera herbicidinsatser på både fältnivå och som ett allmänt planeringsverktyg för rådgivare för att hitta lämpliga tankblandningar och motsvarande doser. Principerna för programmet är baserade på dos-responsdata som härrör från effektförsök. I Danmark pågår för närvarande arbetet med att även använda beslutsstödsprogrammet IPMwise i kombination med artificiell intelligens, automatisk ogräsigenkänning och bekämpningskartor. Denna demo har begränsats när det gäller antalet grödor och ogräs jämfört med den fullständiga danska versionen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demoversion av IPMwise </t>
+  </si>
+  <si>
+    <t>Råd om ogräsbehandling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukauta rikkakasvien hallinta tarpeittesi mukaan joko maanviljelijänä tai neuvojana. Päätä itse, rikkakasvien torjuntataso tai anna IPMwiseen rakennettujen IPM-periaatteiden opastaa sinua. Ohjelmisto sisältää hyödyllisiä työkaluja, joiden avulla voit mukauttaa rikkakasvien torjuntaa ja minimoida rikkakasvien torjunta-aineiden käyttöä. Ohjelmistoa voidaan käyttää rikkakasvien torjunnan suunnitteluun sekä lohkotasolla että yleisenä työkaluna esimerkiksi seosten tai annosnopeuksien suunnittelemiseksi.
+Ohjelman periaatteet perustuvat tehokkuuskokeista saatuihin annosvastetietoihin. Tanskassa työ on parhaillaan käynnissä myös IPMwise-päätöksentukiohjelmiston käyttämiseksi yhdessä tekoälyn, automaattisen rikkakasvien tunnistuksen ja ruiskutuskarttojen kanssa. Tämä versio on rajoitettu koskemaan vaan osaa kasvilajeja ja rikkakasveja verrattuna tanskankieliseen täysversioon.
+</t>
+  </si>
+  <si>
+    <t>IPMwise demoversio</t>
+  </si>
+  <si>
+    <t>Rikkakasvien torjunnan tueksi</t>
+  </si>
+  <si>
+    <t>Piktžolių kontrolę pasirinkite pagal savo, kaip profesionalaus ūkininko ar augalininkystės konsultanto, poreikius. Patys įvertinkite piktžolių kontrolės poreikį arba vadovaukitės IKOK principais naudodami IPMwise. Programinėje įrangoje yra naudingų įrankių, leidžiančių pritaikyti piktžolių kontrolei skirtas priemones atsižvelgiant į piktžolių rūšinę sudėtį lauke ir tai leidžia gerokai sumažinti herbicidų naudojimą. Programinė įranga taip pat gali būti naudojama herbicidų poreikiui planuoti tiek konkretaus lauko lygmeniu, tiek kaip bendrą planavimo įrankį, skirtą konsultantams. Įranga padeda pasirenkant  efektyviausius darbinius mišinius ir tinkamiausias naudojamų herbicidų normas. Programos principai pagrįsti herbicido dozės ir jos atsako duomenimis, gautais iš veiksmingumo ataskaitų. Danijoje šiuo metu taip pat dirbama siekiant naudoti IPMwise sprendimų paramos programinę įrangą kartu su dirbtiniu intelektu, automatiniu piktžolių atpažinimu ir purškimo žemėlapiais. Ši demonstracinė versija yra ribota, palyginti su Danijai tinkama versija, nes apima ribotą augalų ir piktžolių skaičių.</t>
+  </si>
+  <si>
+    <t>IPMwise demo versija</t>
+  </si>
+  <si>
+    <t>Piktžolių kontrolės patarimai</t>
+  </si>
+  <si>
+    <t>Adaptez la gestion de la flore adventice à vos besoins en tant qu'agriculteur ou conseiller agricole. Décidez vous-même du niveau de lutte contre la flore adventice ou laissez-vous guider par les principes de protection intégrée d'IPMwise. Le logiciel contient des outils utiles pour adapter la stratégie de lutte à la population de mauvaises herbes dans un champ et ainsi minimiser considérablement l'utilisation d'herbicides. Le logiciel peut être utilisé pour planifier les stratégies herbicides à la parcelle, et comme un outil de planification général pour les conseillers en culture afin de trouver des mélanges d’herbicides appropriés et les doses correspondantes.
+Les principes du programme sont fondés sur les données de la relation dose-réponse tirées des études d'efficacité. Au Danemark, des travaux sont en cours pour utiliser également le logiciel d'aide à la décision IPMwise en conjonction avec l'intelligence artificielle, la reconnaissance automatique des espèces adventices et les cartes de pulvérisation.
+Cette démo a été limitée pour le nombre de cultures et d’espèces adventices par rapport à la version danoise complète.</t>
+  </si>
+  <si>
+    <t>Version de démonstration d'IPMwise</t>
+  </si>
+  <si>
+    <t>Conseils pour le traitement des mauvaises herbes</t>
+  </si>
+  <si>
+    <t>Personalizzate la gestione delle infestanti secondo le vostre esigenze di agricoltori professionisti o di consulenti colturali. Decidete voi stessi il livello di controllo delle infestanti 
+o lasciatevi guidare dai principi IPM integrati di IPMwise. Il software contiene strumenti utili per adattare lo sforzo contro le infestanti alla 
+popolazione attuale di erbe infestanti in un campo e quindi ridurre notevolmente l'uso di erbicidi. Il software può essere utilizzato per pianificare gli sforzi 
+sia a livello di campo che come strumento di pianificazione generale per i consulenti colturali, per trovare le miscele adatte e le dosi corrispondenti. 
+I principi del programma si basano su dati di risposta alla dose derivati da rapporti di efficacia. In Danimarca si sta lavorando per 
+utilizzare il software di supporto decisionale IPMwise insieme all'intelligenza artificiale, al riconoscimento automatico delle infestanti e alle mappe di irrorazione. 
+Questa demo è stata limitata per quanto riguarda il numero di colture e infestanti rispetto alla versione completa danese.</t>
+  </si>
+  <si>
+    <t>IPMWise versione demo</t>
+  </si>
+  <si>
+    <t>Consigli per il trattamento delle erbe infestanti</t>
+  </si>
+  <si>
+    <t>Προσαρμόστε τη διαχείριση ζιζανίων στις ανάγκες σας ως επαγγελματίας αγρότης ή σύμβουλος καλλιεργειών. Αποφασίστε μόνοι σας το επίπεδο ελέγχου των ζιζανίων ή αφήστε τις ενσωματωμένες αρχές IPM του IPMwise να σας καθοδηγήσουν. Το πρόγραμμα περιέχει χρήσιμα εργαλεία για την προσαρμογή της προσπάθειας κατά των ζιζανίων στις τρέχοντα πληθυσμό ζιζανίων σε έναν αγρό και έτσι να ελαχιστοποιήσετε σημαντικά τη χρήση ζιζανιοκτόνων. Το πρόγραμμα μπορεί να χρησιμοποιηθεί για τον προγραμματισμό ζιζανιοκτόνων προσπαθειών τόσο σε επίπεδο αγρού όσο και ως γενικό εργαλείο σχεδιασμού για τους συμβούλους καλλιέργειας για την εύρεση κατάλληλων μιγμάτων δεξαμενών και αντίστοιχων δόσεων. Οι αρχές του προγράμματος βασίζονται σε δεδομένα απόκρισης δόσης που προέρχονται από εκθέσεις αποτελεσματικότητας. Στη Δανία, διεξάγονται επί του παρόντος εργασίες για χρήση του προγράμματος σε συνδυασμό με τεχνητή νοημοσύνη, αυτόματη αναγνώριση ζιζανίων και χάρτες ψεκασμού.</t>
+  </si>
+  <si>
+    <t>Έκδοση επίδειξης IPMwise</t>
+  </si>
+  <si>
+    <t>Συμβουλές αντιμετώπισης ζιζανίων</t>
   </si>
   <si>
     <t>com.ipmwise.4.models.ipmwiseDK.description</t>
@@ -126,6 +237,68 @@
     <t>IPMwise Denmark</t>
   </si>
   <si>
+    <t>IPMwise Danmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passt das Unkrautmanagement an Ihre Bedürfnisse als professioneller Landwirt oder Anbauberater an. Entscheiden Sie selbst über den Grad der Unkrautbekämpfung oder lassen Sie sich von den integrierten IPM-Grundsätzen von IPMwise leiten. Die Software enthält nützliche Werkzeuge zur Anpassung der Unkrautbekämpfung an die Unkrautpopulation in einem Feld, um so den Einsatz von Herbiziden erheblich zu minimieren. Die Software kann sowohl zur Planung des Herbizideinsatzes auf Feldebene als auch als allgemeines Planungsinstrument für Pflanzenbauberater verwendet werden, um geeignete Tankmischungen und entsprechende Dosierungen zu finden. Die Grundsätze des Programms beruhen auf Dosis-Wirkungs-Daten, die aus Wirksamkeitsberichten abgeleitet werden. In Dänemark wird derzeit daran gearbeitet, die IPMwise-Entscheidungshilfe-Software in Verbindung mit künstlicher Intelligenz, automatischer Unkrauterkennung und Spritzkarten einzusetzen. </t>
+  </si>
+  <si>
+    <t>Stem het onkruidbeheer af op uw behoeften als professionele landbouwer of gewasadviseur. Bepaal zelf het niveau van onkruidbestrijding of laat u leiden door de ingebouwde IPM-beginselen van IPMwise. Het programma bevat nuttige hulpmiddelen om de inspanning tegen onkruid aan te passen aan de huidige onkruidpopulatie in een veld en zo het gebruik van herbiciden aanzienlijk te minimaliseren. Het programma kan worden gebruikt voor het plannen van herbiciden bespuitingen op zowel veldniveau als voor een algemene planningstool voor gewasadviseurs om geschikte tankmixen en bijbehorende doseringen te vinden. 
+De uitgangspunten van het programma zijn gebaseerd op doseringsgegevens uit effectiviteitsrapporten. In Denemarken wordt momenteel gewerkt aan 
+het programma ook te gebruiken in combinatie met kunstmatige intelligentie, automatische onkruidherkenning en spuitkaarten.</t>
+  </si>
+  <si>
+    <t>IPMwise Denemarken</t>
+  </si>
+  <si>
+    <t>Prilagodite obvladovanje plevela svojim potrebam. Sami se odločite o stopnji zatiranja plevela, ali pa se prepustite vgrajenim načelom IPMwise. Programska oprema vsebuje uporabna orodja, s katerimi lahko ukrep proti plevelu prilagodite trenutni stopnji zapleveljenosti in tako znatno zmanjšate uporabo herbicidov. Programsko opremo lahko uporabite za načrtovanje tretiranja s herbicidi tako na ravni polja ali kot splošno orodje za načrtovanje primerne škropilne mešanice in ustrezne odmerke za kmetijske svetovalce. Načela orodja temeljijo na podatkih o odzivu na odmerek, pridobljenih iz poročil o učinkovitosti. Na Danskem trenutno poteka delo za uporabo sistema za podporo odločanju IPMwise v povezavi z umetno inteligenco, samodejnim prepoznavanjem plevela in zemljevidi škropljenja.</t>
+  </si>
+  <si>
+    <t>IPMwise Danska</t>
+  </si>
+  <si>
+    <t>Svetovanje glede zatiranja plevelov</t>
+  </si>
+  <si>
+    <t>Råd om ugrasbekjempelse</t>
+  </si>
+  <si>
+    <t>Anpassa ogräshanteringen efter dina behov som professionell lantbrukare eller rådgivare. Bestäm själv nivån på ogräsbekämpning eller låt de inbyggda IPM-principerna i IPMwise vägleda dig. Programvaran innehåller användbara verktyg för att anpassa ogräsbekämpningen till den aktuella ogräspopulationen i ett fält och därmed en minimerad användning av herbicider. Programvaran kan användas för att planera herbicidinsatser på både fältnivå och som ett allmänt planeringsverktyg för rådgivare för att hitta lämpliga tankblandningar och motsvarande doser. Principerna för programmet är baserade på dos-responsdata som härrör från effektförsök. I Danmark pågår för närvarande arbetet med att även använda beslutsstödsprogrammet IPMwise i kombination med artificiell intelligens, automatisk ogräsigenkänning och bekämpningskartor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapt weed management to your needs as a professional farmer or crop advisor. Decide yourself, the level of weed control 
+or let the built-in IPM principles of IPMwise guide you. The program contains useful tools to adapt the effort against weeds to the 
+current weed population in a field and thus minimize the use of herbicides considerably. The program can be used to plan herbicide 
+efforts at both field level and as a general planning tool for crop advisors to find suitable tank mixtures and corresponding dose rates. 
+The principles of the program are based on dose response data derived from efficacy reports. In Denmark, work is currently underway to 
+also use the program in conjunction with artificial intelligence, automatic weed recognition and spray maps.
+</t>
+  </si>
+  <si>
+    <t>IPMwise Tanska</t>
+  </si>
+  <si>
+    <t>Adaptez la gestion de la flore adventice à vos besoins en tant qu'agriculteur ou conseiller agricole. Décidez vous-même du niveau de lutte contre la flore adventice ou laissez-vous guider par les principes de protection intégrée d'IPMwise. Le logiciel contient des outils utiles pour adapter la stratégie de lutte à la population de mauvaises herbes dans un champ et ainsi minimiser considérablement l'utilisation d'herbicides. Le logiciel peut être utilisé pour planifier les stratégies herbicides à la parcelle, et comme un outil de planification général pour les conseillers en culture afin de trouver des mélanges d’herbicides appropriés et les doses correspondantes.
+Les principes du programme sont fondés sur les données de la relation dose-réponse tirées des études d'efficacité. Au Danemark, des travaux sont en cours pour utiliser également le logiciel d'aide à la décision IPMwise en conjonction avec l'intelligence artificielle, la reconnaissance automatique des espèces adventices et les cartes de pulvérisation.</t>
+  </si>
+  <si>
+    <t>IPMwise Danemark</t>
+  </si>
+  <si>
+    <t>Personalizzate la gestione delle infestanti secondo le vostre esigenze di agricoltori professionisti o di consulenti colturali. Decidete voi stessi il livello di controllo delle infestanti 
+o lasciatevi guidare dai principi IPM integrati di IPMwise. Il programma contiene strumenti utili per adattare lo sforzo contro le infestanti alla 
+popolazione attuale di erbe infestanti in un campo e quindi ridurre notevolmente l'uso di erbicidi. Il programma può essere utilizzato per pianificare gli sforzi 
+sia a livello di campo che come strumento di pianificazione generale per i consulenti colturali, per trovare le miscele adatte e le dosi corrispondenti. 
+I principi del programma si basano su dati di risposta alla dose derivati da rapporti di efficacia. In Danimarca si sta attualmente lavorando per 
+utilizzare il programma anche in combinazione con l'intelligenza artificiale, il riconoscimento automatico delle erbe infestanti e le mappe di irrorazione.</t>
+  </si>
+  <si>
+    <t>IPMwise Danimarca</t>
+  </si>
+  <si>
+    <t>IPMwise Δανία</t>
+  </si>
+  <si>
     <t>com.ipmwise.4.models.ipmwiseES.description</t>
   </si>
   <si>
@@ -148,6 +321,45 @@
     <t>IPMwise Spain</t>
   </si>
   <si>
+    <t>Passt das Unkrautmanagement an Ihre Bedürfnisse als professioneller Landwirt oder Anbauberater an. Entscheiden Sie selbst über den Grad der Unkrautbekämpfung oder lassen Sie sich von den integrierten IPM-Grundsätzen von IPMwise leiten. Die Software enthält nützliche Werkzeuge zur Anpassung der Unkrautbekämpfung an die Unkrautpopulation in einem Feld, um so den Einsatz von Herbiziden erheblich zu minimieren. Die Software kann sowohl zur Planung des Herbizideinsatzes auf Feldebene als auch als allgemeines Planungsinstrument für Pflanzenbauberater verwendet werden, um geeignete Tankmischungen und entsprechende Dosierungen zu finden. Die Grundsätze des Programms beruhen auf Dosis-Wirkungs-Daten, die aus Wirksamkeitsberichten abgeleitet werden. In Dänemark wird derzeit daran gearbeitet, die IPMwise-Entscheidungshilfe-Software in Verbindung mit künstlicher Intelligenz, automatischer Unkrauterkennung und Spritzkarten einzusetzen.</t>
+  </si>
+  <si>
+    <t>IPMwise Spanien</t>
+  </si>
+  <si>
+    <t>Stemt uw onkruidbeheer af op uw behoeften als professionele landbouwer of gewasadviseur. 
+Bepaal zelf het niveau van onkruidbestrijding of gebruik de op IPMwise gebaseerde module om u te begeleiden. 
+Belangrijkste kenmerken: De geïntegreerde tools in IPMWise kunnen u helpen bij het plannen en bepalen van de beste onkruidbestrijdingsstrategieën. 
+De beste onkruidbestrijdingsstrategieën voor uw bedrijf. U kunt simuleren hoe verschillende percelen de omstandigheden de noodzaak tot bestrijding en de beschikbare hulpmiddelen beïnvloeden. Indien u niet beschikt over specifieke aanbevelingen voor de bestrijding van uw onkruid op een bepaald tijdstip, kunt u met IPMWise simuleren of het mogelijk is uw onkruidplagen vóór of na het huidige tijdstip te bestrijden.</t>
+  </si>
+  <si>
+    <t>IPMwise Spanje</t>
+  </si>
+  <si>
+    <t>IPMwise Španija</t>
+  </si>
+  <si>
+    <t>IPMwise Spania</t>
+  </si>
+  <si>
+    <t>Personalizzate la gestione delle infestanti in base alle vostre esigenze di agricoltori professionisti o di consulenti colturali. 
+Decidete voi stessi il livello di controllo delle infestanti o utilizzate il modulo IPMwise per orientarvi. 
+Caratteristiche principali: gli strumenti integrati di IPMWise possono aiutarvi a pianificare e decidere le migliori strategie di controllo delle infestanti. 
+le migliori strategie di controllo delle infestanti per la vostra azienda agricola. È possibile simulare come le diverse condizioni dell'appezzamento
+Le condizioni influiscono sulla necessità di controllo e sugli strumenti disponibili. Nel caso in cui non si disponga di 
+raccomandazioni specifiche per il controllo delle erbe infestanti in un determinato momento, IPMWise vi permette di simulare se in un momento precedente o successivo 
+simulare la possibilità di controllare le infestazioni prima o dopo l'ora corrente.</t>
+  </si>
+  <si>
+    <t>IPMwise Spagna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Προσαρμόστε τη διαχείριση των ζιζανίων στις ανάγκες σας ως επαγγελματίας αγρότης ή σύμβουλος καλλιέργειας. Αποφασίστε μόνοι σας το επίπεδο ελέγχου των ζιζανίων ή χρησιμοποιήστε την ενότητα IPMwise που βασίζεται στη IPM για να σας καθοδηγήσει.  Βασικά χαρακτηριστικά: Τα ενσωματωμένα εργαλεία στο IPMWise μπορούν να σας βοηθήσουν στο σχεδιασμό και τη λήψη απόφασης για τις τις καλύτερες στρατηγικές ελέγχου ζιζανίων για την εκμετάλλευσή σας. Μπορείτε να προσομοιώσετε τον τρόπο με τον οποίο διαφορετικές συνθήκες στο αγροτεμάχιοσυνθήκες επηρεάζουν την ανάγκη για έλεγχο και τα διαθέσιμα εργαλεία. συνθήκες επηρεάζουν την ανάγκη για έλεγχο και τα διαθέσιμα εργαλεία. Σε περίπτωση που δεν έχετε συγκεκριμένες συστάσεις για τον έλεγχο των ζιζανίων σας σε οποιαδήποτε δεδομένη στιγμή, το IPMWise σας επιτρέπει να προσομοιώσετε αν σε προγενέστερες ή μεταγενέστερες προσομοιώσει εάν σε χρονικές στιγμές πριν ή μετά την τρέχουσα χρονική στιγμή είναι δυνατόν να ελέγξετε τις προσβολές των ζιζανίων σας.  </t>
+  </si>
+  <si>
+    <t>IPMwise Ισπανία</t>
+  </si>
+  <si>
     <t>com.ipmwise.4.models.ipmwiseNO.description</t>
   </si>
   <si>
@@ -167,6 +379,62 @@
   </si>
   <si>
     <t>VIPS-ugras Norway</t>
+  </si>
+  <si>
+    <t>VIPS-Ugras 2.0 er en ny version af VIPS-ugras. IPM Consult har udviklet systemet kaldet IPMwise på dansk. Systemet er tilpasset norske forhold af Norsk Institutt for Bioøkonomi (NIBIO) i samarbejde med Norsk Landbrugsrådgivning (NLR). Der er nye beregninger og justeringer, men det er hovedsageligt det samme indhold som i det gamle VIPS-Ugras. VIPS-Ugras 2.0 kræver login. Fordelen ved at logge ind er, at systemet husker dine felter. Systemet er gratis i Norge. Du kan vælge at bruge allerede indtastede effektkrav eller vælge dine egne effektkrav. For en optimal plantebeskyttelsesløsning til de fleste forhold anbefaler vi, at du bruger systemets krav.</t>
+  </si>
+  <si>
+    <t>VIPS-ugras Norge</t>
+  </si>
+  <si>
+    <t>Råd om ukrudtsbehandling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIPS-Ugras 2.0 ist eine neue Version von VIPS-Ugras. IPM Consult hat das System entwickelt, das auf Dänisch IPMwise heißt. 
+Es wurde vom Norwegischen Institut für Bioökonomie (NIBIO) in Zusammenarbeit mit Norsk Landbruksrådgiving (NLR) an norwegische Verhältnisse angepasst. 
+Es gibt neue Berechnungen und Anpassungen, aber der Inhalt ist weitgehend derselbe wie bei den alten VIPS-Ugras. VIPS-Ugras 2.0 erfordert eine Anmeldung. Das Einloggen hat den Vorteil, dass sich das System Ihre Dienste merken kann. Das System ist in Norwegen gebührenfrei. Sie können wählen zwischen dem Verwenden von vorgegebenen Ausgabebedingungen oder wählen Sie Ihre eigenen Ausgabebedingungen. Für eine optimale Pflanzenschutzlösung für die meisten Bedingungen empfehlen wir Ihnen, die Ausgabebedingungen des Systems zu verwenden </t>
+  </si>
+  <si>
+    <t>VIPS-ugras Norwegen</t>
+  </si>
+  <si>
+    <t>VIPS-Ugras 2.0 is een nieuwe versie van VIPS-Ugras. IPM Consult heeft het systeem ontwikkeld, dat in het Deens IPMwise heet. Het is aangepast aan de Noorse omstandigheden door het Noorse Instituut voor bio-economie (NIBIO) in samenwerking met Norsk Landbruksrådgiving (NLR). Er zijn nieuwe berekeningen en aanpassingen gedaan, maar het bevat grotendeels dezelfde inhoud als het oude VIPS-Ugras. VIPS-Ugras 2.0 vereist inloggen. Het voordeel van inloggen is dat het systeem uw diensten kan onthouden. Het systeem is gratis in Noorwegen. U kunt ervoor kiezen om gebruik maken van vooraf ingevoerde uitgangseisen of uw eigen uitgangseisen te kiezen. Voor een optimale gewasbeschermingsoplossing voor de meeste omstandigheden raden wij u aan de uitgangseisen van het systeem te gebruiken.</t>
+  </si>
+  <si>
+    <t>VIPS-ugras Noorwegen</t>
+  </si>
+  <si>
+    <t>Advies over onkruidbehandeling</t>
+  </si>
+  <si>
+    <t>VIPS-Ugras 2.0 je nova različica VIPS-Ugras. IPM Consult je razvil sistem, ki se v danščini imenuje IPMwise. Norveškim razmeram ga je prilagodil Norveški inštitut za bioekonomijo (NIBIO) v sodelovanju z Norveško kmetijsko svetovalno službo (NLR). Obstajajo novi izračuni in prilagoditve, vendar je vsebina skoraj enaka starim VIPS-Ugras. VIPS-Ugras 2.0 zahteva prijavo. Prednost prijave je, da si sistem lahko zapomni vaše podatke. Sistem je na Norveškem brezplačen. Lahko se odločite za uporabo že pripravljenih zahtev glede porabe energije ali izberete lastne zahteve glede porabe energije. Za optimalno rešitev za zaščito rastlin za večino pogojev priporočamo, da uporabite sistemske zahteve za napajanje</t>
+  </si>
+  <si>
+    <t>IPMwise Norveška</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPS-Ugras 2.0 er en ny versjon av VIPS-ugras. IPM Consult har utviklet systemet og som på dansk heter IPMwise. 
+Det er tilpasset norske forhold av Norsk institutt for bioøkonomi (NIBIO) i samarbeid med Norsk Landbruksrådgiving (NLR). 
+Det er nye beregninger og tilpasninger, men det er mye det samme innholdet som gamle VIPS-Ugras. VIPS-Ugras 2.0 krever 
+innlogging. Fordelen med innlogging er at systemet kan huske skiftene dine. Systemet er gratis i Norge. Du kan velge å 
+bruke ferdig innlagte effektkrav eller velge dine egne effektkrav. For en optimal plantevernløsning for de fleste forhold 
+anbefaler vi at du bruker systemets effektkrav  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIPS-Ugras 2.0 är en ny version av VIPS-ugras. IPM Consult har utvecklat systemet som heter IPMwise på danska. Systemet har anpassats till norska förhållanden av Norsk institutt for bioøkonomi (NIBIO) i samarbete med Norsk Landbruksrådgiving (NLR). Det finns nya beräkningar och anpassningar men det är huvudsakligen samma innehåll som i gamla VIPS-Ugras. VIPS-Ugras 2.0 kräver inlogging. Fördelen med inlogging är att systemet kommer ihåg dina fält. Systemet är gratis i Norge. Du kan välja att använda redan inlagda effektkrav eller välja dina egna effektkrav. För en optimal växtskyddslösning för de flesta förhållanden rekommenderar vi att du använder systemets effektkrav.  </t>
+  </si>
+  <si>
+    <t>VIPS rikkakasvit Norja</t>
+  </si>
+  <si>
+    <t>VIPS-ugras Norvegia</t>
+  </si>
+  <si>
+    <t>Το VIPS-Ugras 2.0 είναι μια νέα έκδοση του VIPS-Ugras. Η IPM Consult έχει αναπτύξει το σύστημα, το οποίο στα δανικά ονομάζεται IPMwise.</t>
+  </si>
+  <si>
+    <t>VIPS-ugras Νορβηγία</t>
   </si>
 </sst>
 </file>
@@ -587,6 +855,36 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -653,26 +951,125 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -740,26 +1137,116 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -827,26 +1314,98 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -914,26 +1473,101 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>